<commit_message>
잡스킬 구현, 버그 수정(StatModDiscrete Setter)
</commit_message>
<xml_diff>
--- a/Documents/스킬 정리시트.xlsx
+++ b/Documents/스킬 정리시트.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\DungeonTycoon\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\dungeontycoon\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4430ED76-487D-47F2-8A99-EB6E906F334D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3BCDB50-C66F-48A1-A8DA-3F169D1DD6AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{4E6108CF-2D64-4829-BB95-F44359F74968}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4E6108CF-2D64-4829-BB95-F44359F74968}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="233">
   <si>
     <t>수치</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -279,10 +279,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>사정거리 +1, (나의 최대 사정거리-공격대상과의 거리)*0.15만큼의 공격력 보너스</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>축복</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -291,10 +287,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>입힌 데미지의 15%. 방어막은 방어력이 적용되지 않음.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>별의 심장</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -950,6 +942,25 @@
   </si>
   <si>
     <t>적을 공격할 때마다 공격 대상 양 옆의 적에게 공격력의 35%만큼 피해를 줍니다.</t>
+  </si>
+  <si>
+    <t>Bless</t>
+  </si>
+  <si>
+    <t>적을 공격할 때마다 입힌 피해의 12%에 해당하는 방어막을 얻습니다. 방어막은 3초 동안 지속됩니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사정거리가 1 증가합니다. 가까이 있는 적을 공격할 때 추가 공격력을 얻습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Buckshot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사정거리 +1, (나의 최대 사정거리-공격대상과의 거리)*0.1만큼의 공격력 보너스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1363,8 +1374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF457FC-3F16-4162-AAFC-4292C4AB5A29}">
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1385,25 +1396,25 @@
         <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>24</v>
@@ -1418,10 +1429,10 @@
         <v>33</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.4">
@@ -1429,31 +1440,31 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>8</v>
@@ -1463,173 +1474,173 @@
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>218</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>26</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M3" s="1"/>
       <c r="N3" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>37</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="K4" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>37</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>26</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>40</v>
       </c>
       <c r="M6" s="1"/>
       <c r="N6" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="52.2" x14ac:dyDescent="0.4">
@@ -1637,29 +1648,29 @@
         <v>57</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>227</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
         <v>58</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>59</v>
@@ -1669,7 +1680,7 @@
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="52.2" x14ac:dyDescent="0.4">
@@ -1677,29 +1688,29 @@
         <v>44</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
         <v>45</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>46</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>43</v>
@@ -1709,70 +1720,86 @@
       </c>
       <c r="M8" s="1"/>
       <c r="N8" s="9" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.4">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>229</v>
+      </c>
       <c r="D9" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>26</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>40</v>
       </c>
       <c r="M9" s="1"/>
+      <c r="N9" s="9" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="10" spans="1:14" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>230</v>
+      </c>
       <c r="D10" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>26</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>61</v>
+        <v>232</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1" t="s">
         <v>40</v>
       </c>
       <c r="M10" s="1"/>
+      <c r="N10" s="9" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="11" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
@@ -1780,17 +1807,17 @@
       </c>
       <c r="B11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
         <v>37</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>27</v>
@@ -1812,23 +1839,23 @@
       </c>
       <c r="B12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
         <v>37</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>42</v>
@@ -1838,7 +1865,7 @@
       </c>
       <c r="M12" s="1"/>
       <c r="N12" s="9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.4">
@@ -1847,23 +1874,23 @@
       </c>
       <c r="B13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
         <v>37</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>51</v>
@@ -1873,7 +1900,7 @@
       </c>
       <c r="M13" s="1"/>
       <c r="N13" s="9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.4">
@@ -1882,25 +1909,25 @@
       </c>
       <c r="B14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>56</v>
@@ -1909,24 +1936,24 @@
         <v>40</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1" t="s">
@@ -1934,406 +1961,406 @@
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
         <v>45</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K16" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="J16" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="L16" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M16" s="1"/>
     </row>
     <row r="17" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="4" t="s">
         <v>45</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M17" s="1"/>
     </row>
     <row r="18" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>26</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M18" s="1"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B19" s="1"/>
       <c r="D19" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
         <v>37</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M19" s="1"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B20" s="1"/>
       <c r="D20" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
         <v>37</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M20" s="1"/>
     </row>
     <row r="21" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
         <v>37</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M21" s="1"/>
     </row>
     <row r="22" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A22" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>26</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="N22" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="87" x14ac:dyDescent="0.4">
       <c r="A23" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>26</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="M23" s="1"/>
       <c r="N23" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A24" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
         <v>45</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I24" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="L24" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="M24" s="1"/>
       <c r="N24" s="9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="87" x14ac:dyDescent="0.4">
       <c r="A25" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>151</v>
-      </c>
       <c r="G25" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="M25" s="1"/>
       <c r="N25" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="87" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>37</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I26" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="K26" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="J26" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="L26" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="M26" s="1"/>
       <c r="N26" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.4">
@@ -2342,19 +2369,19 @@
       </c>
       <c r="B27" s="1"/>
       <c r="D27" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>53</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>26</v>
@@ -2376,19 +2403,19 @@
       </c>
       <c r="B28" s="1"/>
       <c r="D28" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>45</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>25</v>
@@ -2410,19 +2437,19 @@
       </c>
       <c r="B29" s="1"/>
       <c r="D29" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>26</v>
@@ -2444,149 +2471,149 @@
       </c>
       <c r="B30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E30" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>174</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>26</v>
       </c>
       <c r="J30" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="L30" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="L30" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="M30" s="1"/>
     </row>
     <row r="31" spans="1:14" ht="156.6" x14ac:dyDescent="0.4">
       <c r="A31" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J31" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="K31" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="M31" s="1"/>
       <c r="N31" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A32" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J32" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F32" s="1" t="s">
+      <c r="K32" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G32" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>163</v>
-      </c>
       <c r="L32" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="M32" s="1"/>
       <c r="N32" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B33" s="1"/>
       <c r="D33" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E33" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="G33" s="1" t="s">
+      <c r="I33" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="K33" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="L33" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M33" s="1"/>
     </row>
@@ -2596,17 +2623,17 @@
       </c>
       <c r="B34" s="1"/>
       <c r="D34" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>26</v>
@@ -2624,33 +2651,33 @@
     </row>
     <row r="35" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B35" s="1"/>
       <c r="D35" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M35" s="1"/>
     </row>
@@ -2663,22 +2690,22 @@
         <v>14</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>37</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>27</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>15</v>
@@ -2697,17 +2724,17 @@
         <v>29</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1" t="s">
         <v>48</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>49</v>
@@ -2729,14 +2756,14 @@
         <v>29</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>26</v>
@@ -2761,14 +2788,14 @@
         <v>29</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>26</v>
@@ -2786,81 +2813,81 @@
     </row>
     <row r="40" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A40" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B40" s="1"/>
       <c r="D40" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M40" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="J40" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="L40" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="M40" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="M41" s="1"/>
       <c r="N41" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A42" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -2868,14 +2895,14 @@
         <v>29</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>26</v>
@@ -2887,7 +2914,7 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A43" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -2899,19 +2926,19 @@
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="M43" s="1"/>
       <c r="N43" s="9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A44" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -2923,14 +2950,14 @@
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="M44" s="1"/>
       <c r="N44" s="9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>